<commit_message>
Add single send to contacts
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mihranw\Desktop\Tools\Email Sender\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mihranw\Desktop\Tools\Email Sender\Group-MailSender\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1125E980-D7AE-480E-A124-3B00E3AAF987}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A48A4793-483C-446A-8A25-0A01BF599E40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25180" windowHeight="16140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>mihranw@gmail.com</t>
   </si>
@@ -36,7 +36,13 @@
     <t>Email</t>
   </si>
   <si>
-    <t>parzhangi@gmail.com</t>
+    <t>1380.9.15@gmail.com</t>
+  </si>
+  <si>
+    <t>hasan.com</t>
+  </si>
+  <si>
+    <t>irnic.mihranw@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -365,10 +371,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -396,11 +402,22 @@
         <v>3</v>
       </c>
     </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{DE2A85CA-EDD0-4A97-9A0C-8CCE69FBE389}"/>
     <hyperlink ref="A3" r:id="rId2" xr:uid="{F04159B7-ABA3-4927-81F5-C1B9367EEFBE}"/>
     <hyperlink ref="A4" r:id="rId3" xr:uid="{32D766B6-18B4-4578-B731-65C05C29387B}"/>
+    <hyperlink ref="A6" r:id="rId4" xr:uid="{2C22CA90-5393-40D3-A99D-EFCE53D909BA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update and add requirements
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mihranw\Desktop\Tools\Email Sender\Group-MailSender\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A48A4793-483C-446A-8A25-0A01BF599E40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B069F60-DE02-465A-A2C9-8262FA3490B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25180" windowHeight="16140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>mihranw@gmail.com</t>
   </si>
@@ -43,6 +43,9 @@
   </si>
   <si>
     <t>irnic.mihranw@gmail.com</t>
+  </si>
+  <si>
+    <t>regenerative.md@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -371,10 +374,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -412,13 +415,20 @@
         <v>5</v>
       </c>
     </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{DE2A85CA-EDD0-4A97-9A0C-8CCE69FBE389}"/>
     <hyperlink ref="A3" r:id="rId2" xr:uid="{F04159B7-ABA3-4927-81F5-C1B9367EEFBE}"/>
     <hyperlink ref="A4" r:id="rId3" xr:uid="{32D766B6-18B4-4578-B731-65C05C29387B}"/>
     <hyperlink ref="A6" r:id="rId4" xr:uid="{2C22CA90-5393-40D3-A99D-EFCE53D909BA}"/>
+    <hyperlink ref="A7" r:id="rId5" display="mailto:regenerative.md@gmail.com" xr:uid="{72FB704B-299B-476D-BFD6-86280B6913CB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>